<commit_message>
Export with dummy header
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+  <si>
+    <t>Name</t>
+  </si>
   <si>
     <t>Anuraj Shetty</t>
   </si>
@@ -478,7 +481,7 @@
   <s:sheetPr>
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
   </s:sheetPr>
-  <dimension ref="A2:A44"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,219 +489,224 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>